<commit_message>
feat: open u 题库
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiayi/PycharmProjects/simulateRobot/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2E7853-026B-C04C-A7C2-B41F5134EC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12380" yWindow="1300" windowWidth="20500" windowHeight="7860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="14600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22">
   <si>
     <t>序号</t>
   </si>
@@ -40,25 +34,34 @@
     <t>陶山</t>
   </si>
   <si>
+    <t>130533198207254834</t>
+  </si>
+  <si>
     <t>汽车运用与维修技术</t>
   </si>
   <si>
     <t>胡月</t>
   </si>
   <si>
+    <t>422827198803241829</t>
+  </si>
+  <si>
     <t>会计</t>
   </si>
   <si>
     <t>郝旭</t>
   </si>
   <si>
+    <t>422827198409231868</t>
+  </si>
+  <si>
     <t>工商企业管理</t>
   </si>
   <si>
     <t>谭进</t>
   </si>
   <si>
-    <t>1942001463847</t>
+    <t>429005199101161401</t>
   </si>
   <si>
     <t>行政管理</t>
@@ -67,26 +70,29 @@
     <t>吴思儒</t>
   </si>
   <si>
-    <t>1942001463849</t>
-  </si>
-  <si>
-    <t>130533198207254834</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>422827198803241829</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>422827198409231868</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <t>42900519920323136X</t>
+  </si>
+  <si>
+    <t>吴睿</t>
+  </si>
+  <si>
+    <t>422201198607166810</t>
+  </si>
+  <si>
+    <t>xxx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,34 +103,362 @@
     <font>
       <sz val="10"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -160,15 +494,260 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -185,18 +764,68 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
+    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
+    <cellStyle name="输入" xfId="4" builtinId="20"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
+    <cellStyle name="货币" xfId="7" builtinId="4"/>
+    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
+    <cellStyle name="百分比" xfId="9" builtinId="5"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
+    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
+    <cellStyle name="计算" xfId="15" builtinId="22"/>
+    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
+    <cellStyle name="适中" xfId="17" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
+    <cellStyle name="好" xfId="19" builtinId="26"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="差" xfId="22" builtinId="27"/>
+    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
+    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
+    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
+    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
+    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
+    <cellStyle name="标题" xfId="33" builtinId="15"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
+    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="注释" xfId="37" builtinId="10"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
+    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8"/>
+    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
+    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
+    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -454,129 +1083,147 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="6" outlineLevelCol="4"/>
   <cols>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1"/>
-    <col min="5" max="5" width="22.1640625" customWidth="1"/>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="3" max="3" width="20.1826923076923" customWidth="1"/>
+    <col min="4" max="4" width="15.6634615384615" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.1634615384615" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15">
-      <c r="A2" s="2">
+    <row r="2" spans="1:5">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>12345678</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="5">
+        <v>12345678</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="5">
+        <v>12345678</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="5">
+        <v>12345678</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="2">
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="5">
         <v>12345678</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E6" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" ht="17" spans="1:5">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="4">
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1">
         <v>12345678</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="4">
-        <v>12345678</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="4">
-        <v>19950924</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="4">
-        <v>19921029</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>13</v>
+      <c r="E7" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>